<commit_message>
Aplicación de formatos sobre el reporte Excel y detección de tipo de plantilla
</commit_message>
<xml_diff>
--- a/recursos/formatos/upiicsa.xlsx
+++ b/recursos/formatos/upiicsa.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="75" windowWidth="15480" windowHeight="6360"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">LLENADO!$A$1:$AG$43</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1986,16 +1986,16 @@
     <t>DEPENDENCIA DONDE REALIZA SU SERVICIO SOCIAL:</t>
   </si>
   <si>
-    <t>REPORTE MENSUAL DE SERVICIO SOCIAL =</t>
-  </si>
-  <si>
-    <t>CONTROL DE ASISTENCIAS =</t>
-  </si>
-  <si>
     <t>SELLO DE RECIBIDO D. E. y A. E. UPIICSA</t>
   </si>
   <si>
     <t>RESPONSABLE DIRECTO DE SUPERVSION DE SERVICIO SOCIAL:</t>
+  </si>
+  <si>
+    <t>CONTROL DE ASISTENCIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPORTE MENSUAL DE SERVICIO SOCIAL </t>
   </si>
 </sst>
 </file>
@@ -2243,10 +2243,10 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2255,7 +2255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2354,9 +2354,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2369,11 +2366,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2387,12 +2421,20 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2406,20 +2448,98 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -2429,133 +2549,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2670,13 +2664,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>112060</xdr:colOff>
+      <xdr:colOff>123266</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>205113</xdr:colOff>
+      <xdr:colOff>216319</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -2702,8 +2696,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5244354" y="57150"/>
-          <a:ext cx="608524" cy="733425"/>
+          <a:off x="12001501" y="57150"/>
+          <a:ext cx="619730" cy="654984"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2738,13 +2732,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>15688</xdr:colOff>
+      <xdr:colOff>71718</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>46264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>310963</xdr:colOff>
+      <xdr:colOff>366993</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>27214</xdr:rowOff>
     </xdr:to>
@@ -2770,8 +2764,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10792545" y="46264"/>
-          <a:ext cx="635454" cy="742950"/>
+          <a:off x="5272368" y="46264"/>
+          <a:ext cx="590550" cy="666750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2803,88 +2797,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>16</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>142875</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Object 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>361950</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Object 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>52579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="7 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6010276" y="28575"/>
+          <a:ext cx="514350" cy="709804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>52579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="8 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76201" y="28575"/>
+          <a:ext cx="514350" cy="709804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3177,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12:Z12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3213,187 +3213,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61" t="s">
+      <c r="A1" s="78"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="61" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="72"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="62"/>
-      <c r="AA3" s="62"/>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="62"/>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="62"/>
-      <c r="AF3" s="72"/>
-      <c r="AG3" s="72"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
     </row>
     <row r="4" spans="1:33" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
-      <c r="V4" s="62"/>
-      <c r="W4" s="62"/>
-      <c r="X4" s="62"/>
-      <c r="Y4" s="62"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="62"/>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="62"/>
-      <c r="AD4" s="62"/>
-      <c r="AE4" s="62"/>
-      <c r="AF4" s="72"/>
-      <c r="AG4" s="72"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="88" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="88"/>
-      <c r="Y5" s="88"/>
-      <c r="Z5" s="88"/>
-      <c r="AA5" s="88"/>
-      <c r="AB5" s="88"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
+      <c r="A5" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="60"/>
+      <c r="W5" s="60"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="60"/>
+      <c r="AB5" s="60"/>
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="60"/>
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -3446,33 +3446,33 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="65" t="s">
+      <c r="L7" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="68">
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="85">
         <f>E14</f>
         <v>0</v>
       </c>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
-      <c r="V7" s="68"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="85"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="85"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="85"/>
+      <c r="X7" s="85"/>
+      <c r="Y7" s="85"/>
+      <c r="Z7" s="85"/>
+      <c r="AA7" s="85"/>
       <c r="AB7" s="20"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
-      <c r="AE7" s="66"/>
-      <c r="AF7" s="66"/>
-      <c r="AG7" s="66"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
     </row>
     <row r="8" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -3519,56 +3519,56 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="36" t="s">
+      <c r="Q9" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="87" t="s">
+      <c r="R9" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="87"/>
-      <c r="T9" s="87"/>
-      <c r="U9" s="87" t="s">
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="87"/>
-      <c r="W9" s="87"/>
-      <c r="X9" s="87" t="s">
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="Y9" s="87"/>
-      <c r="Z9" s="87"/>
-      <c r="AA9" s="87" t="s">
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="AB9" s="87"/>
-      <c r="AC9" s="87"/>
-      <c r="AD9" s="89" t="s">
+      <c r="AB9" s="61"/>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="AE9" s="90"/>
-      <c r="AF9" s="90"/>
-      <c r="AG9" s="91"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="67"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="35"/>
@@ -3581,22 +3581,22 @@
       <c r="Q10" s="21">
         <v>1</v>
       </c>
-      <c r="R10" s="59"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="75"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="68"/>
       <c r="V10" s="76"/>
       <c r="W10" s="77"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="45"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="47"/>
-      <c r="AB10" s="47"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="47"/>
-      <c r="AE10" s="47"/>
-      <c r="AF10" s="47"/>
-      <c r="AG10" s="47"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="55"/>
+      <c r="Z10" s="56"/>
+      <c r="AA10" s="48"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="48"/>
+      <c r="AG10" s="48"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -3608,56 +3608,56 @@
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="36" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="O11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="37" t="s">
+      <c r="P11" s="36" t="s">
         <v>15</v>
       </c>
       <c r="Q11" s="21">
         <v>2</v>
       </c>
-      <c r="R11" s="59"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="49"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="51"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="47"/>
-      <c r="AB11" s="47"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="47"/>
-      <c r="AE11" s="47"/>
-      <c r="AF11" s="47"/>
-      <c r="AG11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="63"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="55"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="48"/>
+      <c r="AB11" s="48"/>
+      <c r="AC11" s="48"/>
+      <c r="AD11" s="48"/>
+      <c r="AE11" s="48"/>
+      <c r="AF11" s="48"/>
+      <c r="AG11" s="48"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -3669,22 +3669,22 @@
       <c r="Q12" s="21">
         <v>3</v>
       </c>
-      <c r="R12" s="59"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="45"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="47"/>
-      <c r="AB12" s="47"/>
-      <c r="AC12" s="47"/>
-      <c r="AD12" s="47"/>
-      <c r="AE12" s="47"/>
-      <c r="AF12" s="47"/>
-      <c r="AG12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="63"/>
+      <c r="W12" s="64"/>
+      <c r="X12" s="54"/>
+      <c r="Y12" s="55"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="48"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -3706,63 +3706,63 @@
       <c r="Q13" s="21">
         <v>4</v>
       </c>
-      <c r="R13" s="59"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="49"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="47"/>
-      <c r="AD13" s="47"/>
-      <c r="AE13" s="47"/>
-      <c r="AF13" s="47"/>
-      <c r="AG13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="64"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="55"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="48"/>
+      <c r="AC13" s="48"/>
+      <c r="AD13" s="48"/>
+      <c r="AE13" s="48"/>
+      <c r="AF13" s="48"/>
+      <c r="AG13" s="48"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="69" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="69"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="90"/>
       <c r="Q14" s="21">
         <v>5</v>
       </c>
-      <c r="R14" s="59"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="49"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="63"/>
+      <c r="W14" s="64"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="55"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="48"/>
+      <c r="AB14" s="48"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="48"/>
+      <c r="AE14" s="48"/>
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="48"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -3784,61 +3784,61 @@
       <c r="Q15" s="21">
         <v>6</v>
       </c>
-      <c r="R15" s="75"/>
-      <c r="S15" s="78"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="46"/>
-      <c r="AA15" s="47"/>
-      <c r="AB15" s="47"/>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="47"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="47"/>
-      <c r="AG15" s="47"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="70"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="64"/>
+      <c r="X15" s="54"/>
+      <c r="Y15" s="55"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="48"/>
+      <c r="AB15" s="48"/>
+      <c r="AC15" s="48"/>
+      <c r="AD15" s="48"/>
+      <c r="AE15" s="48"/>
+      <c r="AF15" s="48"/>
+      <c r="AG15" s="48"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="42">
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="21">
         <v>7</v>
       </c>
-      <c r="R16" s="75"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="47"/>
-      <c r="AB16" s="47"/>
-      <c r="AC16" s="47"/>
-      <c r="AD16" s="47"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="47"/>
-      <c r="AG16" s="47"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="69"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="64"/>
+      <c r="X16" s="54"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="48"/>
+      <c r="AF16" s="48"/>
+      <c r="AG16" s="48"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -3860,43 +3860,43 @@
       <c r="Q17" s="21">
         <v>8</v>
       </c>
-      <c r="R17" s="75"/>
-      <c r="S17" s="78"/>
-      <c r="T17" s="79"/>
-      <c r="U17" s="49"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="47"/>
-      <c r="AB17" s="47"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="47"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="47"/>
-      <c r="AG17" s="47"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="69"/>
+      <c r="T17" s="70"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="63"/>
+      <c r="W17" s="64"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="55"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="48"/>
+      <c r="AC17" s="48"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="48"/>
+      <c r="AF17" s="48"/>
+      <c r="AG17" s="48"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Q18" s="21">
         <v>9</v>
       </c>
-      <c r="R18" s="75"/>
-      <c r="S18" s="78"/>
-      <c r="T18" s="79"/>
-      <c r="U18" s="49"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="46"/>
-      <c r="AA18" s="47"/>
-      <c r="AB18" s="47"/>
-      <c r="AC18" s="47"/>
-      <c r="AD18" s="47"/>
-      <c r="AE18" s="47"/>
-      <c r="AF18" s="47"/>
-      <c r="AG18" s="47"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="69"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="63"/>
+      <c r="W18" s="64"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="55"/>
+      <c r="Z18" s="56"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="48"/>
+      <c r="AC18" s="48"/>
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="48"/>
+      <c r="AF18" s="48"/>
+      <c r="AG18" s="48"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -3910,166 +3910,166 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
       <c r="Q19" s="21">
         <v>10</v>
       </c>
-      <c r="R19" s="75"/>
-      <c r="S19" s="78"/>
-      <c r="T19" s="79"/>
-      <c r="U19" s="49"/>
-      <c r="V19" s="50"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="47"/>
-      <c r="AB19" s="47"/>
-      <c r="AC19" s="47"/>
-      <c r="AD19" s="47"/>
-      <c r="AE19" s="47"/>
-      <c r="AF19" s="47"/>
-      <c r="AG19" s="47"/>
+      <c r="R19" s="68"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="63"/>
+      <c r="W19" s="64"/>
+      <c r="X19" s="54"/>
+      <c r="Y19" s="55"/>
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="48"/>
+      <c r="AB19" s="48"/>
+      <c r="AC19" s="48"/>
+      <c r="AD19" s="48"/>
+      <c r="AE19" s="48"/>
+      <c r="AF19" s="48"/>
+      <c r="AG19" s="48"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="71"/>
-      <c r="O20" s="71"/>
-      <c r="P20" s="71"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
+      <c r="O20" s="88"/>
+      <c r="P20" s="88"/>
       <c r="Q20" s="21">
         <v>11</v>
       </c>
-      <c r="R20" s="59"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="49"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="46"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="47"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="47"/>
-      <c r="AE20" s="47"/>
-      <c r="AF20" s="47"/>
-      <c r="AG20" s="47"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="63"/>
+      <c r="W20" s="64"/>
+      <c r="X20" s="54"/>
+      <c r="Y20" s="55"/>
+      <c r="Z20" s="56"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
+      <c r="AF20" s="48"/>
+      <c r="AG20" s="48"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
       <c r="Q21" s="21">
         <v>12</v>
       </c>
-      <c r="R21" s="59"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="46"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
-      <c r="AC21" s="47"/>
-      <c r="AD21" s="47"/>
-      <c r="AE21" s="47"/>
-      <c r="AF21" s="47"/>
-      <c r="AG21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="62"/>
+      <c r="V21" s="63"/>
+      <c r="W21" s="64"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="56"/>
+      <c r="AA21" s="48"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="48"/>
+      <c r="AD21" s="48"/>
+      <c r="AE21" s="48"/>
+      <c r="AF21" s="48"/>
+      <c r="AG21" s="48"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Q22" s="21">
         <v>13</v>
       </c>
-      <c r="R22" s="59"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="50"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="47"/>
-      <c r="AB22" s="47"/>
-      <c r="AC22" s="47"/>
-      <c r="AD22" s="47"/>
-      <c r="AE22" s="47"/>
-      <c r="AF22" s="47"/>
-      <c r="AG22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="63"/>
+      <c r="W22" s="64"/>
+      <c r="X22" s="54"/>
+      <c r="Y22" s="55"/>
+      <c r="Z22" s="56"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="48"/>
+      <c r="AF22" s="48"/>
+      <c r="AG22" s="48"/>
     </row>
     <row r="23" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
+      <c r="A23" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="43"/>
+      <c r="P23" s="7"/>
       <c r="Q23" s="21">
         <v>14</v>
       </c>
-      <c r="R23" s="59"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="47"/>
-      <c r="U23" s="49"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="44"/>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="47"/>
-      <c r="AB23" s="47"/>
-      <c r="AC23" s="47"/>
-      <c r="AD23" s="47"/>
-      <c r="AE23" s="47"/>
-      <c r="AF23" s="47"/>
-      <c r="AG23" s="47"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="64"/>
+      <c r="X23" s="54"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="56"/>
+      <c r="AA23" s="48"/>
+      <c r="AB23" s="48"/>
+      <c r="AC23" s="48"/>
+      <c r="AD23" s="48"/>
+      <c r="AE23" s="48"/>
+      <c r="AF23" s="48"/>
+      <c r="AG23" s="48"/>
     </row>
     <row r="24" spans="1:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
@@ -4089,182 +4089,187 @@
       <c r="Q24" s="21">
         <v>15</v>
       </c>
-      <c r="R24" s="59"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="49"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="44"/>
-      <c r="Y24" s="45"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="47"/>
-      <c r="AB24" s="47"/>
-      <c r="AC24" s="47"/>
-      <c r="AD24" s="47"/>
-      <c r="AE24" s="47"/>
-      <c r="AF24" s="47"/>
-      <c r="AG24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="62"/>
+      <c r="V24" s="63"/>
+      <c r="W24" s="64"/>
+      <c r="X24" s="54"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="56"/>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="48"/>
+      <c r="AC24" s="48"/>
+      <c r="AD24" s="48"/>
+      <c r="AE24" s="48"/>
+      <c r="AF24" s="48"/>
+      <c r="AG24" s="48"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="92"/>
+      <c r="O25" s="92"/>
+      <c r="P25" s="92"/>
       <c r="Q25" s="21">
         <v>16</v>
       </c>
-      <c r="R25" s="59"/>
-      <c r="S25" s="47"/>
-      <c r="T25" s="47"/>
-      <c r="U25" s="49"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="44"/>
-      <c r="Y25" s="45"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="47"/>
-      <c r="AB25" s="47"/>
-      <c r="AC25" s="47"/>
-      <c r="AD25" s="47"/>
-      <c r="AE25" s="47"/>
-      <c r="AF25" s="47"/>
-      <c r="AG25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="48"/>
+      <c r="U25" s="62"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="64"/>
+      <c r="X25" s="54"/>
+      <c r="Y25" s="55"/>
+      <c r="Z25" s="56"/>
+      <c r="AA25" s="48"/>
+      <c r="AB25" s="48"/>
+      <c r="AC25" s="48"/>
+      <c r="AD25" s="48"/>
+      <c r="AE25" s="48"/>
+      <c r="AF25" s="48"/>
+      <c r="AG25" s="48"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="92"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="92"/>
+      <c r="P26" s="92"/>
       <c r="Q26" s="21">
         <v>17</v>
       </c>
-      <c r="R26" s="59"/>
-      <c r="S26" s="47"/>
-      <c r="T26" s="47"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="50"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="47"/>
-      <c r="AB26" s="47"/>
-      <c r="AC26" s="47"/>
-      <c r="AD26" s="47"/>
-      <c r="AE26" s="47"/>
-      <c r="AF26" s="47"/>
-      <c r="AG26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="48"/>
+      <c r="T26" s="48"/>
+      <c r="U26" s="62"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="64"/>
+      <c r="X26" s="54"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="56"/>
+      <c r="AA26" s="48"/>
+      <c r="AB26" s="48"/>
+      <c r="AC26" s="48"/>
+      <c r="AD26" s="48"/>
+      <c r="AE26" s="48"/>
+      <c r="AF26" s="48"/>
+      <c r="AG26" s="48"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="L27" s="55" t="s">
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="J27" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="M27" s="55"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
       <c r="Q27" s="21">
         <v>18</v>
       </c>
-      <c r="R27" s="59"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="49"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="44"/>
-      <c r="Y27" s="45"/>
-      <c r="Z27" s="46"/>
-      <c r="AA27" s="47"/>
-      <c r="AB27" s="47"/>
-      <c r="AC27" s="47"/>
-      <c r="AD27" s="47"/>
-      <c r="AE27" s="47"/>
-      <c r="AF27" s="47"/>
-      <c r="AG27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="64"/>
+      <c r="X27" s="54"/>
+      <c r="Y27" s="55"/>
+      <c r="Z27" s="56"/>
+      <c r="AA27" s="48"/>
+      <c r="AB27" s="48"/>
+      <c r="AC27" s="48"/>
+      <c r="AD27" s="48"/>
+      <c r="AE27" s="48"/>
+      <c r="AF27" s="48"/>
+      <c r="AG27" s="48"/>
     </row>
     <row r="28" spans="1:33" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q28" s="21">
         <v>19</v>
       </c>
-      <c r="R28" s="59"/>
-      <c r="S28" s="47"/>
-      <c r="T28" s="47"/>
-      <c r="U28" s="49"/>
-      <c r="V28" s="50"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="44"/>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="46"/>
-      <c r="AA28" s="47"/>
-      <c r="AB28" s="47"/>
-      <c r="AC28" s="47"/>
-      <c r="AD28" s="47"/>
-      <c r="AE28" s="47"/>
-      <c r="AF28" s="47"/>
-      <c r="AG28" s="47"/>
+      <c r="R28" s="47"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+      <c r="U28" s="62"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="64"/>
+      <c r="X28" s="54"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="56"/>
+      <c r="AA28" s="48"/>
+      <c r="AB28" s="48"/>
+      <c r="AC28" s="48"/>
+      <c r="AD28" s="48"/>
+      <c r="AE28" s="48"/>
+      <c r="AF28" s="48"/>
+      <c r="AG28" s="48"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="91"/>
+      <c r="P29" s="91"/>
       <c r="Q29" s="21">
         <v>20</v>
       </c>
-      <c r="R29" s="59"/>
-      <c r="S29" s="47"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="49"/>
-      <c r="V29" s="50"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="45"/>
-      <c r="Z29" s="46"/>
-      <c r="AA29" s="47"/>
-      <c r="AB29" s="47"/>
-      <c r="AC29" s="47"/>
-      <c r="AD29" s="47"/>
-      <c r="AE29" s="47"/>
-      <c r="AF29" s="47"/>
-      <c r="AG29" s="47"/>
+      <c r="R29" s="47"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+      <c r="U29" s="62"/>
+      <c r="V29" s="63"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="54"/>
+      <c r="Y29" s="55"/>
+      <c r="Z29" s="56"/>
+      <c r="AA29" s="48"/>
+      <c r="AB29" s="48"/>
+      <c r="AC29" s="48"/>
+      <c r="AD29" s="48"/>
+      <c r="AE29" s="48"/>
+      <c r="AF29" s="48"/>
+      <c r="AG29" s="48"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -4286,237 +4291,237 @@
       <c r="Q30" s="21">
         <v>21</v>
       </c>
-      <c r="R30" s="59"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="49"/>
-      <c r="V30" s="50"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="44"/>
-      <c r="Y30" s="45"/>
-      <c r="Z30" s="46"/>
-      <c r="AA30" s="47"/>
-      <c r="AB30" s="47"/>
-      <c r="AC30" s="47"/>
-      <c r="AD30" s="47"/>
-      <c r="AE30" s="47"/>
-      <c r="AF30" s="47"/>
-      <c r="AG30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="62"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="64"/>
+      <c r="X30" s="54"/>
+      <c r="Y30" s="55"/>
+      <c r="Z30" s="56"/>
+      <c r="AA30" s="48"/>
+      <c r="AB30" s="48"/>
+      <c r="AC30" s="48"/>
+      <c r="AD30" s="48"/>
+      <c r="AE30" s="48"/>
+      <c r="AF30" s="48"/>
+      <c r="AG30" s="48"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>1</v>
       </c>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-      <c r="N31" s="83"/>
-      <c r="O31" s="83"/>
-      <c r="P31" s="83"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
       <c r="Q31" s="21">
         <v>22</v>
       </c>
-      <c r="R31" s="59"/>
-      <c r="S31" s="47"/>
-      <c r="T31" s="47"/>
-      <c r="U31" s="49"/>
-      <c r="V31" s="50"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="44"/>
-      <c r="Y31" s="45"/>
-      <c r="Z31" s="46"/>
-      <c r="AA31" s="47"/>
-      <c r="AB31" s="47"/>
-      <c r="AC31" s="47"/>
-      <c r="AD31" s="47"/>
-      <c r="AE31" s="47"/>
-      <c r="AF31" s="47"/>
-      <c r="AG31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="62"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="64"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="55"/>
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="48"/>
+      <c r="AC31" s="48"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="48"/>
+      <c r="AF31" s="48"/>
+      <c r="AG31" s="48"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>2</v>
       </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
       <c r="Q32" s="21">
         <v>23</v>
       </c>
-      <c r="R32" s="59"/>
-      <c r="S32" s="47"/>
-      <c r="T32" s="47"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="45"/>
-      <c r="W32" s="46"/>
-      <c r="X32" s="44"/>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="46"/>
-      <c r="AA32" s="47"/>
-      <c r="AB32" s="47"/>
-      <c r="AC32" s="47"/>
-      <c r="AD32" s="47"/>
-      <c r="AE32" s="47"/>
-      <c r="AF32" s="47"/>
-      <c r="AG32" s="47"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="48"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="56"/>
+      <c r="X32" s="54"/>
+      <c r="Y32" s="55"/>
+      <c r="Z32" s="56"/>
+      <c r="AA32" s="48"/>
+      <c r="AB32" s="48"/>
+      <c r="AC32" s="48"/>
+      <c r="AD32" s="48"/>
+      <c r="AE32" s="48"/>
+      <c r="AF32" s="48"/>
+      <c r="AG32" s="48"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>3</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
       <c r="Q33" s="21">
         <v>24</v>
       </c>
-      <c r="R33" s="59"/>
-      <c r="S33" s="47"/>
-      <c r="T33" s="47"/>
-      <c r="U33" s="44"/>
-      <c r="V33" s="45"/>
-      <c r="W33" s="46"/>
-      <c r="X33" s="44"/>
-      <c r="Y33" s="45"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="47"/>
-      <c r="AB33" s="47"/>
-      <c r="AC33" s="47"/>
-      <c r="AD33" s="47"/>
-      <c r="AE33" s="47"/>
-      <c r="AF33" s="47"/>
-      <c r="AG33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="55"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="54"/>
+      <c r="Y33" s="55"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="48"/>
+      <c r="AB33" s="48"/>
+      <c r="AC33" s="48"/>
+      <c r="AD33" s="48"/>
+      <c r="AE33" s="48"/>
+      <c r="AF33" s="48"/>
+      <c r="AG33" s="48"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>4</v>
       </c>
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-      <c r="M34" s="86"/>
-      <c r="N34" s="86"/>
-      <c r="O34" s="86"/>
-      <c r="P34" s="86"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
       <c r="Q34" s="21">
         <v>25</v>
       </c>
-      <c r="R34" s="59"/>
-      <c r="S34" s="47"/>
-      <c r="T34" s="47"/>
-      <c r="U34" s="44"/>
-      <c r="V34" s="45"/>
-      <c r="W34" s="46"/>
-      <c r="X34" s="44"/>
-      <c r="Y34" s="45"/>
-      <c r="Z34" s="46"/>
-      <c r="AA34" s="47"/>
-      <c r="AB34" s="47"/>
-      <c r="AC34" s="47"/>
-      <c r="AD34" s="47"/>
-      <c r="AE34" s="47"/>
-      <c r="AF34" s="47"/>
-      <c r="AG34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="48"/>
+      <c r="T34" s="48"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="56"/>
+      <c r="X34" s="54"/>
+      <c r="Y34" s="55"/>
+      <c r="Z34" s="56"/>
+      <c r="AA34" s="48"/>
+      <c r="AB34" s="48"/>
+      <c r="AC34" s="48"/>
+      <c r="AD34" s="48"/>
+      <c r="AE34" s="48"/>
+      <c r="AF34" s="48"/>
+      <c r="AG34" s="48"/>
     </row>
     <row r="35" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>5</v>
       </c>
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="86"/>
-      <c r="O35" s="86"/>
-      <c r="P35" s="86"/>
-      <c r="Q35" s="81" t="s">
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="R35" s="81"/>
-      <c r="S35" s="81"/>
-      <c r="T35" s="81"/>
-      <c r="U35" s="81"/>
-      <c r="V35" s="81"/>
-      <c r="W35" s="81"/>
-      <c r="X35" s="81"/>
-      <c r="Y35" s="81"/>
-      <c r="Z35" s="81"/>
-      <c r="AA35" s="95">
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="50"/>
+      <c r="V35" s="50"/>
+      <c r="W35" s="50"/>
+      <c r="X35" s="50"/>
+      <c r="Y35" s="50"/>
+      <c r="Z35" s="50"/>
+      <c r="AA35" s="52">
         <f>SUM(AA10:AC34)</f>
         <v>0</v>
       </c>
-      <c r="AB35" s="95"/>
-      <c r="AC35" s="95"/>
-      <c r="AD35" s="96"/>
-      <c r="AE35" s="96"/>
-      <c r="AF35" s="96"/>
-      <c r="AG35" s="96"/>
+      <c r="AB35" s="52"/>
+      <c r="AC35" s="52"/>
+      <c r="AD35" s="53"/>
+      <c r="AE35" s="53"/>
+      <c r="AF35" s="53"/>
+      <c r="AG35" s="53"/>
     </row>
     <row r="36" spans="1:34" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="Q36" s="81" t="s">
+      <c r="Q36" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="R36" s="81"/>
-      <c r="S36" s="81"/>
-      <c r="T36" s="81"/>
-      <c r="U36" s="81"/>
-      <c r="V36" s="81"/>
-      <c r="W36" s="81"/>
-      <c r="X36" s="81"/>
-      <c r="Y36" s="81"/>
-      <c r="Z36" s="81"/>
-      <c r="AA36" s="94"/>
-      <c r="AB36" s="94"/>
-      <c r="AC36" s="94"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="50"/>
+      <c r="AA36" s="51"/>
+      <c r="AB36" s="51"/>
+      <c r="AC36" s="51"/>
       <c r="AD36" s="15"/>
       <c r="AE36" s="15"/>
       <c r="AF36" s="15"/>
@@ -4529,9 +4534,9 @@
       <c r="K37" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L37" s="84"/>
-      <c r="M37" s="84"/>
-      <c r="N37" s="84"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
       <c r="O37" s="6" t="s">
         <v>24</v>
       </c>
@@ -4540,37 +4545,37 @@
     <row r="38" spans="1:34" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:34" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="Q40" s="82"/>
-      <c r="R40" s="82"/>
-      <c r="S40" s="82"/>
-      <c r="T40" s="82"/>
-      <c r="U40" s="82"/>
-      <c r="V40" s="82"/>
-      <c r="X40" s="38"/>
-      <c r="Y40" s="39"/>
-      <c r="Z40" s="39"/>
-      <c r="AA40" s="39"/>
-      <c r="AC40" s="39"/>
-      <c r="AD40" s="39"/>
-      <c r="AE40" s="39"/>
-      <c r="AF40" s="39"/>
-      <c r="AG40" s="39"/>
+      <c r="A40" s="89"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="Q40" s="94"/>
+      <c r="R40" s="94"/>
+      <c r="S40" s="94"/>
+      <c r="T40" s="94"/>
+      <c r="U40" s="94"/>
+      <c r="V40" s="94"/>
+      <c r="X40" s="37"/>
+      <c r="Y40" s="38"/>
+      <c r="Z40" s="38"/>
+      <c r="AA40" s="38"/>
+      <c r="AC40" s="38"/>
+      <c r="AD40" s="38"/>
+      <c r="AE40" s="38"/>
+      <c r="AF40" s="38"/>
+      <c r="AG40" s="38"/>
     </row>
     <row r="41" spans="1:34" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
@@ -4580,14 +4585,14 @@
       <c r="N41"/>
       <c r="O41"/>
       <c r="P41"/>
-      <c r="Q41" s="85" t="s">
+      <c r="Q41" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="R41" s="85"/>
-      <c r="S41" s="85"/>
-      <c r="T41" s="85"/>
-      <c r="U41" s="85"/>
-      <c r="V41" s="85"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="73"/>
+      <c r="V41" s="73"/>
       <c r="X41" s="8"/>
       <c r="Y41" s="8"/>
       <c r="Z41" s="8"/>
@@ -4598,94 +4603,254 @@
       <c r="AG41" s="8"/>
     </row>
     <row r="42" spans="1:34" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="80">
+      <c r="A42" s="43">
         <f>B25</f>
         <v>0</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
-      <c r="H42" s="92"/>
-      <c r="I42" s="92"/>
-      <c r="J42" s="92"/>
-      <c r="K42" s="92"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
       <c r="L42"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="80">
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="43">
         <f>B25</f>
         <v>0</v>
       </c>
-      <c r="R42" s="80"/>
-      <c r="S42" s="80"/>
-      <c r="T42" s="80"/>
-      <c r="U42" s="80"/>
-      <c r="V42" s="80"/>
-      <c r="X42" s="92"/>
-      <c r="Y42" s="92"/>
-      <c r="Z42" s="92"/>
-      <c r="AA42" s="92"/>
-      <c r="AC42" s="40"/>
-      <c r="AD42" s="40"/>
-      <c r="AE42" s="40"/>
-      <c r="AF42" s="40"/>
-      <c r="AG42" s="40"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="44"/>
+      <c r="Z42" s="44"/>
+      <c r="AA42" s="44"/>
+      <c r="AC42" s="39"/>
+      <c r="AD42" s="39"/>
+      <c r="AE42" s="39"/>
+      <c r="AF42" s="39"/>
+      <c r="AG42" s="39"/>
       <c r="AH42" s="8"/>
     </row>
     <row r="43" spans="1:34" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="80">
+      <c r="A43" s="43">
         <f>J25</f>
         <v>0</v>
       </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
-      <c r="H43" s="93" t="s">
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="H43" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
       <c r="L43"/>
-      <c r="M43" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" s="93"/>
-      <c r="O43" s="93"/>
-      <c r="P43" s="93"/>
-      <c r="Q43" s="80">
+      <c r="M43" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="N43" s="45"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="43">
         <f>J25</f>
         <v>0</v>
       </c>
-      <c r="R43" s="80"/>
-      <c r="S43" s="80"/>
-      <c r="T43" s="80"/>
-      <c r="U43" s="80"/>
-      <c r="V43" s="80"/>
-      <c r="X43" s="93" t="s">
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="X43" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="Y43" s="93"/>
-      <c r="Z43" s="93"/>
-      <c r="AA43" s="93"/>
-      <c r="AC43" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD43" s="93"/>
-      <c r="AE43" s="93"/>
-      <c r="AF43" s="93"/>
-      <c r="AG43" s="41"/>
-      <c r="AH43" s="41"/>
+      <c r="Y43" s="45"/>
+      <c r="Z43" s="45"/>
+      <c r="AA43" s="45"/>
+      <c r="AC43" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD43" s="45"/>
+      <c r="AE43" s="45"/>
+      <c r="AF43" s="45"/>
+      <c r="AG43" s="40"/>
+      <c r="AH43" s="40"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="185">
+  <mergeCells count="184">
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="AD25:AG25"/>
+    <mergeCell ref="AD26:AG26"/>
+    <mergeCell ref="AD27:AG27"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AA31:AC31"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="X29:Z29"/>
+    <mergeCell ref="AA29:AC29"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="X27:Z27"/>
+    <mergeCell ref="AA27:AC27"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="AD28:AG28"/>
+    <mergeCell ref="AA30:AC30"/>
+    <mergeCell ref="AA26:AC26"/>
+    <mergeCell ref="AD29:AG29"/>
+    <mergeCell ref="AA28:AC28"/>
+    <mergeCell ref="X30:Z30"/>
+    <mergeCell ref="X26:Z26"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="J25:P26"/>
+    <mergeCell ref="B25:H26"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="Q35:Z35"/>
+    <mergeCell ref="Q40:V40"/>
+    <mergeCell ref="X28:Z28"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="X34:Z34"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:N4"/>
+    <mergeCell ref="O1:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="AD17:AG17"/>
+    <mergeCell ref="AD18:AG18"/>
+    <mergeCell ref="AD19:AG19"/>
+    <mergeCell ref="AD20:AG20"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="AD14:AG14"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="Q7:AA7"/>
+    <mergeCell ref="AC7:AG7"/>
+    <mergeCell ref="AA13:AC13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="A20:P20"/>
+    <mergeCell ref="Q1:R4"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="AA25:AC25"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="X23:Z23"/>
+    <mergeCell ref="AA23:AC23"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="X25:Z25"/>
+    <mergeCell ref="AA24:AC24"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B33:P33"/>
+    <mergeCell ref="B34:P34"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="AD15:AG15"/>
+    <mergeCell ref="AD16:AG16"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="B31:P31"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="Q41:V41"/>
+    <mergeCell ref="R32:T32"/>
+    <mergeCell ref="U32:W32"/>
+    <mergeCell ref="X32:Z32"/>
+    <mergeCell ref="R33:T33"/>
+    <mergeCell ref="U33:W33"/>
+    <mergeCell ref="X33:Z33"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="Q42:V42"/>
+    <mergeCell ref="AD10:AG10"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="AA16:AC16"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="AA15:AC15"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="AD21:AG21"/>
+    <mergeCell ref="AD22:AG22"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AD12:AG12"/>
+    <mergeCell ref="AD13:AG13"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AD24:AG24"/>
+    <mergeCell ref="AF1:AG4"/>
+    <mergeCell ref="S1:AE4"/>
+    <mergeCell ref="Q5:AG5"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="AA21:AC21"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="X22:Z22"/>
+    <mergeCell ref="AA22:AC22"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="X19:Z19"/>
+    <mergeCell ref="AA19:AC19"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="X20:Z20"/>
+    <mergeCell ref="AA20:AC20"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AA14:AC14"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AA9:AC9"/>
+    <mergeCell ref="AD9:AG9"/>
+    <mergeCell ref="AA17:AC17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="AA18:AC18"/>
     <mergeCell ref="Q43:V43"/>
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="X42:AA42"/>
@@ -4710,167 +4875,6 @@
     <mergeCell ref="AD35:AG35"/>
     <mergeCell ref="R34:T34"/>
     <mergeCell ref="U34:W34"/>
-    <mergeCell ref="AF1:AG4"/>
-    <mergeCell ref="S1:AE4"/>
-    <mergeCell ref="Q5:AG5"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="AA21:AC21"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="X22:Z22"/>
-    <mergeCell ref="AA22:AC22"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="X19:Z19"/>
-    <mergeCell ref="AA19:AC19"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="X20:Z20"/>
-    <mergeCell ref="AA20:AC20"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AA14:AC14"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AA9:AC9"/>
-    <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="AA17:AC17"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="AA18:AC18"/>
-    <mergeCell ref="AD15:AG15"/>
-    <mergeCell ref="AD16:AG16"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="AD10:AG10"/>
-    <mergeCell ref="X16:Z16"/>
-    <mergeCell ref="AA16:AC16"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="AA15:AC15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="Q42:V42"/>
-    <mergeCell ref="Q35:Z35"/>
-    <mergeCell ref="Q40:V40"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="X21:Z21"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="X28:Z28"/>
-    <mergeCell ref="B31:P31"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="Q41:V41"/>
-    <mergeCell ref="R32:T32"/>
-    <mergeCell ref="U32:W32"/>
-    <mergeCell ref="X32:Z32"/>
-    <mergeCell ref="R33:T33"/>
-    <mergeCell ref="U33:W33"/>
-    <mergeCell ref="X33:Z33"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B33:P33"/>
-    <mergeCell ref="B34:P34"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R28:T28"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="X26:Z26"/>
-    <mergeCell ref="AA26:AC26"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="X23:Z23"/>
-    <mergeCell ref="AA23:AC23"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="X25:Z25"/>
-    <mergeCell ref="AA24:AC24"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="AA25:AC25"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:N4"/>
-    <mergeCell ref="O1:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="AD17:AG17"/>
-    <mergeCell ref="AD18:AG18"/>
-    <mergeCell ref="AD19:AG19"/>
-    <mergeCell ref="AD20:AG20"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="AD14:AG14"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="Q7:AA7"/>
-    <mergeCell ref="AC7:AG7"/>
-    <mergeCell ref="AA13:AC13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="E14:K14"/>
-    <mergeCell ref="A20:P20"/>
-    <mergeCell ref="Q1:R4"/>
-    <mergeCell ref="AD21:AG21"/>
-    <mergeCell ref="AD22:AG22"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="A29:P29"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="J25:P26"/>
-    <mergeCell ref="B25:H26"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="AD12:AG12"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="AD13:AG13"/>
-    <mergeCell ref="AD29:AG29"/>
-    <mergeCell ref="AA28:AC28"/>
-    <mergeCell ref="X30:Z30"/>
-    <mergeCell ref="X34:Z34"/>
-    <mergeCell ref="AA34:AC34"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AD24:AG24"/>
-    <mergeCell ref="AD25:AG25"/>
-    <mergeCell ref="AD26:AG26"/>
-    <mergeCell ref="AD27:AG27"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="AA31:AC31"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="X29:Z29"/>
-    <mergeCell ref="AA29:AC29"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="X27:Z27"/>
-    <mergeCell ref="AA27:AC27"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AD28:AG28"/>
-    <mergeCell ref="AA30:AC30"/>
-    <mergeCell ref="U26:W26"/>
   </mergeCells>
   <conditionalFormatting sqref="Q7">
     <cfRule type="containsBlanks" dxfId="12" priority="17" stopIfTrue="1">
@@ -4941,58 +4945,6 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="1026" r:id="rId4">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>17</xdr:col>
-                <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="1026" r:id="rId4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="PBrush" shapeId="1027" r:id="rId6">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>361950</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="PBrush" shapeId="1027" r:id="rId6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">

</xml_diff>